<commit_message>
- removed duplicate terms - cleaned up tables
</commit_message>
<xml_diff>
--- a/Excel/Chapter2.xlsx
+++ b/Excel/Chapter2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyaa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyaa\Documents\R project\LDAGlossary\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810E5D37-95EF-45DF-A7B3-637D1A67E341}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502B881E-FDF6-4E51-BDFA-5D69B23215F0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{F38E7673-4FF7-461E-BD5C-C56DA1E24695}"/>
   </bookViews>
@@ -30,12 +30,6 @@
     <t>claim</t>
   </si>
   <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
     <t>expected cost</t>
   </si>
   <si>
@@ -120,6 +114,12 @@
   </si>
   <si>
     <t>compensation from insurer to insured upon the occurrence of an insured event</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>severity</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DCC5EE-78DF-4F5D-AE9B-862FC2ADAB26}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -518,13 +518,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -532,15 +532,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -559,10 +559,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -570,10 +570,10 @@
     </row>
     <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
@@ -581,18 +581,18 @@
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
@@ -600,18 +600,18 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
@@ -619,42 +619,42 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>